<commit_message>
(fase1:)Actualizacion duoc evaluacion individual, actualizacion doc presentacion,avance matriz EDT
</commit_message>
<xml_diff>
--- a/fase1/Documentacion Proyecto/Matriz EDT.xlsb.xlsx
+++ b/fase1/Documentacion Proyecto/Matriz EDT.xlsb.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\git\Capstone\fase1\Documentacion Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74EB88AF-B725-4843-AE3D-6E8F8AAB391A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0555DC3D-2AB2-4F2E-B38E-7BEC0A2FB62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EDT" sheetId="1" r:id="rId1"/>
     <sheet name="Costos Fases" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="94">
   <si>
     <t>Fase de Planificación</t>
   </si>
@@ -320,20 +319,19 @@
   </si>
   <si>
     <t>Camila Rodríguez</t>
-  </si>
-  <si>
-    <t>=</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;$&quot;* #,##0_ ;_ &quot;$&quot;* \-#,##0_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0_ ;\-0\ "/>
+    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,6 +362,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -530,10 +535,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -596,8 +602,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Millares [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -912,7 +921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J58"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
@@ -2000,8 +2009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="64" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView zoomScale="64" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2055,14 +2064,14 @@
       <c r="C3" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="29">
         <v>25000</v>
       </c>
       <c r="E3" s="8">
         <f>EDT!C6+EDT!C7+EDT!C8+EDT!C9</f>
         <v>60</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="29">
         <f>D3*E3</f>
         <v>1500000</v>
       </c>
@@ -2089,23 +2098,29 @@
       <c r="C4" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="29">
         <v>22000</v>
       </c>
       <c r="E4" s="8">
         <f>EDT!D6+EDT!D7+EDT!D8+EDT!D9</f>
         <v>40</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="29">
         <f>D4*E4</f>
         <v>880000</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J4" s="29">
+        <v>25000</v>
+      </c>
+      <c r="K4" s="28">
+        <v>4000000</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -2117,23 +2132,29 @@
       <c r="C5" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="29">
         <v>20000</v>
       </c>
       <c r="E5" s="8">
         <f>EDT!E6+EDT!E7+EDT!E8+EDT!E9</f>
         <v>10</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="29">
         <f>D5*E5</f>
         <v>200000</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="I5" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="J5" s="29">
+        <v>22000</v>
+      </c>
+      <c r="K5" s="29">
+        <v>3520000</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -2145,23 +2166,29 @@
       <c r="C6" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="29">
         <v>18000</v>
       </c>
       <c r="E6" s="8">
         <f>EDT!F6+EDT!F7+EDT!F8+EDT!F9</f>
         <v>20</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="29">
         <f>D6*E6</f>
         <v>360000</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="I6" t="s">
+        <v>91</v>
+      </c>
+      <c r="J6" s="29">
+        <v>20000</v>
+      </c>
+      <c r="K6" s="29">
+        <v>3200000</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -2173,23 +2200,29 @@
       <c r="C7" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="29">
         <v>18000</v>
       </c>
       <c r="E7" s="8">
         <f>EDT!G6+EDT!G7+EDT!G8+EDT!G9</f>
         <v>15</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="29">
         <f>D7*E7</f>
         <v>270000</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="I7" t="s">
+        <v>92</v>
+      </c>
+      <c r="J7" s="29">
+        <v>18000</v>
+      </c>
+      <c r="K7" s="29">
+        <v>2880000</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
@@ -2199,16 +2232,22 @@
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
       <c r="E8" s="27"/>
-      <c r="F8" s="7">
+      <c r="F8" s="29">
         <f>SUM(F3:F7)</f>
         <v>3210000</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="I8" t="s">
+        <v>93</v>
+      </c>
+      <c r="J8" s="29">
+        <v>18000</v>
+      </c>
+      <c r="K8" s="29">
+        <v>2880000</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
@@ -2244,7 +2283,7 @@
       <c r="C12" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="29">
         <v>25000</v>
       </c>
       <c r="E12" s="8">
@@ -2260,7 +2299,7 @@
       </c>
       <c r="I12" s="7">
         <f>F3+F12+F21+F30+F39</f>
-        <v>5625000</v>
+        <v>7125000</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
@@ -2273,7 +2312,7 @@
       <c r="C13" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="29">
         <v>22000</v>
       </c>
       <c r="E13" s="8">
@@ -2287,13 +2326,11 @@
       <c r="H13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="7" t="e">
+      <c r="I13" s="7">
         <f>F4+F13+F22+F31+F40</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L13" s="1">
-        <v>25000</v>
-      </c>
+        <v>13640000</v>
+      </c>
+      <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
@@ -2305,7 +2342,7 @@
       <c r="C14" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="29">
         <v>20000</v>
       </c>
       <c r="E14" s="8">
@@ -2321,7 +2358,7 @@
       </c>
       <c r="I14" s="7">
         <f>F5+F14+F23+F32+F41</f>
-        <v>4000000</v>
+        <v>4700000</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
@@ -2334,7 +2371,7 @@
       <c r="C15" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="29">
         <v>18000</v>
       </c>
       <c r="E15" s="8">
@@ -2350,7 +2387,7 @@
       </c>
       <c r="I15" s="7">
         <f>F6+F15+F24+F33+F42</f>
-        <v>2610000</v>
+        <v>4680000</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
@@ -2363,7 +2400,7 @@
       <c r="C16" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="29">
         <v>18000</v>
       </c>
       <c r="E16" s="8">
@@ -2379,7 +2416,7 @@
       </c>
       <c r="I16" s="7">
         <f>F7+F16+F25+F34+F43</f>
-        <v>2970000</v>
+        <v>4050000</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
@@ -2397,9 +2434,9 @@
       <c r="H17" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="11" t="e">
+      <c r="I17" s="11">
         <f>SUM(I12:I16)</f>
-        <v>#VALUE!</v>
+        <v>34195000</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
@@ -2439,7 +2476,7 @@
       <c r="C21" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="29">
         <v>25000</v>
       </c>
       <c r="E21" s="8">
@@ -2472,7 +2509,7 @@
       <c r="C22" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="29">
         <v>22000</v>
       </c>
       <c r="E22" s="8">
@@ -2501,7 +2538,7 @@
       <c r="C23" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="29">
         <v>20000</v>
       </c>
       <c r="E23" s="8">
@@ -2530,7 +2567,7 @@
       <c r="C24" t="s">
         <v>92</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="29">
         <v>18000</v>
       </c>
       <c r="E24" s="8">
@@ -2544,9 +2581,9 @@
       <c r="H24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I24" s="7" t="e">
+      <c r="I24" s="7">
         <f>F35</f>
-        <v>#VALUE!</v>
+        <v>3800000</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
@@ -2559,7 +2596,7 @@
       <c r="C25" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="29">
         <v>18000</v>
       </c>
       <c r="E25" s="8">
@@ -2575,7 +2612,7 @@
       </c>
       <c r="I25" s="7">
         <f>F44</f>
-        <v>0</v>
+        <v>4360000</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
@@ -2593,9 +2630,9 @@
       <c r="H26" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I26" s="11" t="e">
+      <c r="I26" s="11">
         <f>SUM(I21:I25)</f>
-        <v>#VALUE!</v>
+        <v>34195000</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="29" x14ac:dyDescent="0.35">
@@ -2634,7 +2671,7 @@
       <c r="C30" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="29">
         <v>25000</v>
       </c>
       <c r="E30" s="8">
@@ -2648,9 +2685,9 @@
       <c r="H30" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I30" s="7" t="e">
+      <c r="I30" s="7">
         <f>I26*I29</f>
-        <v>#VALUE!</v>
+        <v>20517000</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
@@ -2663,22 +2700,23 @@
       <c r="C31" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="29">
         <v>22000</v>
       </c>
-      <c r="E31" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="F31" s="7" t="e">
+      <c r="E31" s="8">
+        <f>EDT!D48+EDT!D49+EDT!D50</f>
+        <v>50</v>
+      </c>
+      <c r="F31" s="7">
         <f>D31*E31</f>
-        <v>#VALUE!</v>
+        <v>1100000</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I31" s="7" t="e">
+      <c r="I31" s="7">
         <f>I26+I30</f>
-        <v>#VALUE!</v>
+        <v>54712000</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
@@ -2691,15 +2729,16 @@
       <c r="C32" t="s">
         <v>91</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="29">
         <v>20000</v>
       </c>
       <c r="E32" s="8">
-        <v>0</v>
+        <f>EDT!E48+EDT!E49+EDT!E50</f>
+        <v>20</v>
       </c>
       <c r="F32" s="7">
         <f>D32*E32</f>
-        <v>0</v>
+        <v>400000</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -2712,15 +2751,16 @@
       <c r="C33" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="29">
         <v>18000</v>
       </c>
       <c r="E33" s="8">
-        <v>0</v>
+        <f>EDT!F48+EDT!F49+EDT!F50</f>
+        <v>80</v>
       </c>
       <c r="F33" s="7">
         <f>D33*E33</f>
-        <v>0</v>
+        <v>1440000</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -2733,15 +2773,16 @@
       <c r="C34" t="s">
         <v>93</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="29">
         <v>18000</v>
       </c>
       <c r="E34" s="8">
-        <v>0</v>
+        <f>EDT!G48+EDT!G49+EDT!G50</f>
+        <v>20</v>
       </c>
       <c r="F34" s="7">
         <f>D34*E34</f>
-        <v>0</v>
+        <v>360000</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
@@ -2752,9 +2793,9 @@
       <c r="C35" s="26"/>
       <c r="D35" s="26"/>
       <c r="E35" s="27"/>
-      <c r="F35" s="7" t="e">
+      <c r="F35" s="7">
         <f>SUM(F30:F34)</f>
-        <v>#VALUE!</v>
+        <v>3800000</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -2787,15 +2828,16 @@
       <c r="C39" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39" s="29">
         <v>25000</v>
       </c>
       <c r="E39" s="8">
-        <v>0</v>
+        <f>EDT!C53+EDT!C54+EDT!C55+EDT!C56</f>
+        <v>60</v>
       </c>
       <c r="F39" s="7">
         <f>D39*E39</f>
-        <v>0</v>
+        <v>1500000</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -2808,15 +2850,16 @@
       <c r="C40" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40" s="29">
         <v>22000</v>
       </c>
       <c r="E40" s="8">
-        <v>0</v>
+        <f>EDT!D53+EDT!D54+EDT!D55+EDT!D56</f>
+        <v>55</v>
       </c>
       <c r="F40" s="7">
         <f>D40*E40</f>
-        <v>0</v>
+        <v>1210000</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -2829,15 +2872,16 @@
       <c r="C41" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41" s="29">
         <v>20000</v>
       </c>
       <c r="E41" s="8">
-        <v>0</v>
+        <f>EDT!E53+EDT!E54+EDT!E55+EDT!E56</f>
+        <v>15</v>
       </c>
       <c r="F41" s="7">
         <f>D41*E41</f>
-        <v>0</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -2850,15 +2894,16 @@
       <c r="C42" t="s">
         <v>92</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42" s="29">
         <v>18000</v>
       </c>
       <c r="E42" s="8">
-        <v>0</v>
+        <f>EDT!F53+EDT!F54+EDT!F55+EDT!F56</f>
+        <v>35</v>
       </c>
       <c r="F42" s="7">
         <f>D42*E42</f>
-        <v>0</v>
+        <v>630000</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -2871,15 +2916,16 @@
       <c r="C43" t="s">
         <v>93</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43" s="29">
         <v>18000</v>
       </c>
       <c r="E43" s="8">
-        <v>0</v>
+        <f>EDT!G53+EDT!G54+EDT!G55+EDT!G56</f>
+        <v>40</v>
       </c>
       <c r="F43" s="7">
         <f>D43*E43</f>
-        <v>0</v>
+        <v>720000</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -2892,7 +2938,7 @@
       <c r="E44" s="27"/>
       <c r="F44" s="7">
         <f>SUM(F39:F43)</f>
-        <v>0</v>
+        <v>4360000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(fase1:)Actualizacion duoc evaluacion individual, actualizacion doc EDT
</commit_message>
<xml_diff>
--- a/fase1/Documentacion Proyecto/Matriz EDT.xlsb.xlsx
+++ b/fase1/Documentacion Proyecto/Matriz EDT.xlsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\git\Capstone\fase1\Documentacion Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A997E9-70A9-43C3-A69D-A27C7A61BDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7261F15C-531A-4025-BCAA-84EF27747CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EDT" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="96">
   <si>
     <t>Fase de Planificación</t>
   </si>
@@ -322,6 +322,9 @@
   </si>
   <si>
     <t xml:space="preserve">dias </t>
+  </si>
+  <si>
+    <t>dias esperados</t>
   </si>
 </sst>
 </file>
@@ -410,7 +413,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -538,12 +541,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -564,12 +580,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="42" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -608,7 +618,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares [0]" xfId="1" builtinId="6"/>
@@ -924,490 +945,548 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J58"/>
+  <dimension ref="A2:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="A44" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="49.36328125" customWidth="1"/>
-    <col min="2" max="2" width="7.36328125" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" customWidth="1"/>
-    <col min="5" max="5" width="9.08984375" customWidth="1"/>
-    <col min="6" max="6" width="8.08984375" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="5" customWidth="1"/>
-    <col min="9" max="9" width="23.26953125" customWidth="1"/>
-    <col min="10" max="10" width="29.7265625" customWidth="1"/>
+    <col min="2" max="3" width="7.36328125" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="9.08984375" customWidth="1"/>
+    <col min="7" max="7" width="8.08984375" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="5" customWidth="1"/>
+    <col min="10" max="10" width="23.26953125" customWidth="1"/>
+    <col min="11" max="11" width="29.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="I4" s="23" t="s">
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="J4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="23"/>
-    </row>
-    <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="K4" s="21"/>
+    </row>
+    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>20</v>
+      <c r="C5" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="30">
-        <f>(C6+D6+E6+F6+G6)/8</f>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="33">
+        <f>(D6+E6+F6+G6+H6)/8</f>
         <v>4.375</v>
       </c>
-      <c r="C6" s="4">
-        <v>20</v>
-      </c>
       <c r="D6" s="4">
-        <v>5</v>
-      </c>
-      <c r="E6" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5</v>
+      </c>
       <c r="F6" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G6" s="4">
         <v>5</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>20</v>
+      <c r="H6" s="4">
+        <v>5</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="30">
-        <f t="shared" ref="B7:B56" si="0">(C7+D7+E7+F7+G7)/8</f>
+    <row r="7" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="33">
+        <f>(D7+E7+F7+G7+H7)/8</f>
         <v>2.5</v>
       </c>
-      <c r="C7" s="4">
-        <v>10</v>
-      </c>
       <c r="D7" s="4">
-        <v>5</v>
-      </c>
-      <c r="E7" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="E7" s="4">
+        <v>5</v>
+      </c>
       <c r="F7" s="4">
-        <v>5</v>
-      </c>
-      <c r="G7" s="4"/>
-      <c r="I7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>5</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="K7" s="10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="30">
-        <f t="shared" si="0"/>
+      <c r="B8" s="1">
+        <v>8</v>
+      </c>
+      <c r="C8" s="33">
+        <f>(D8+E8+F8+G8+H8)/8</f>
         <v>7.5</v>
       </c>
-      <c r="C8" s="4">
+      <c r="D8" s="4">
         <v>15</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E8" s="4">
         <v>25</v>
       </c>
-      <c r="E8" s="4">
-        <v>5</v>
-      </c>
       <c r="F8" s="4">
         <v>5</v>
       </c>
       <c r="G8" s="4">
-        <v>10</v>
-      </c>
-      <c r="I8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="4">
+        <v>10</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="30">
-        <f t="shared" si="0"/>
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="33">
+        <f>(D9+E9+F9+G9+H9)/8</f>
         <v>3.75</v>
       </c>
-      <c r="C9" s="4">
+      <c r="D9" s="4">
         <v>15</v>
       </c>
-      <c r="D9" s="4">
-        <v>5</v>
-      </c>
       <c r="E9" s="4">
         <v>5</v>
       </c>
       <c r="F9" s="4">
         <v>5</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="I9" s="1" t="s">
+      <c r="G9" s="4">
+        <v>5</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C10" s="4"/>
+    <row r="10" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="29"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="33"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="I10" s="1" t="s">
+      <c r="H10" s="4"/>
+      <c r="J10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="33"/>
       <c r="D11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="G11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="H11" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
+    <row r="12" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="30">
-        <f t="shared" si="0"/>
+      <c r="B12" s="1">
+        <v>9</v>
+      </c>
+      <c r="C12" s="33">
+        <f>(D12+E12+F12+G12+H12)/8</f>
         <v>8.75</v>
       </c>
-      <c r="C12" s="4">
+      <c r="D12" s="4">
         <v>15</v>
       </c>
-      <c r="D12" s="4">
+      <c r="E12" s="4">
         <v>30</v>
       </c>
-      <c r="E12" s="4">
-        <v>10</v>
-      </c>
       <c r="F12" s="4">
         <v>10</v>
       </c>
       <c r="G12" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="30">
-        <f t="shared" si="0"/>
+      <c r="B13" s="1">
+        <v>8</v>
+      </c>
+      <c r="C13" s="33">
+        <f>(D13+E13+F13+G13+H13)/8</f>
         <v>7.5</v>
       </c>
-      <c r="C13" s="4">
-        <v>10</v>
-      </c>
       <c r="D13" s="4">
+        <v>10</v>
+      </c>
+      <c r="E13" s="4">
         <v>25</v>
       </c>
-      <c r="E13" s="4">
+      <c r="F13" s="4">
         <v>15</v>
       </c>
-      <c r="F13" s="4">
-        <v>5</v>
-      </c>
       <c r="G13" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
+      <c r="H13" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="30">
-        <f t="shared" si="0"/>
+      <c r="B14" s="1">
+        <v>7</v>
+      </c>
+      <c r="C14" s="33">
+        <f>(D14+E14+F14+G14+H14)/8</f>
         <v>6.875</v>
       </c>
-      <c r="C14" s="4">
-        <v>10</v>
-      </c>
       <c r="D14" s="4">
+        <v>10</v>
+      </c>
+      <c r="E14" s="4">
         <v>30</v>
       </c>
-      <c r="E14" s="4"/>
       <c r="F14" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G14" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="30">
-        <f t="shared" si="0"/>
+      <c r="B15" s="1">
+        <v>7</v>
+      </c>
+      <c r="C15" s="33">
+        <f>(D15+E15+F15+G15+H15)/8</f>
         <v>6.875</v>
       </c>
-      <c r="C15" s="4">
-        <v>5</v>
-      </c>
       <c r="D15" s="4">
-        <v>10</v>
-      </c>
-      <c r="E15" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="E15" s="4">
+        <v>10</v>
+      </c>
       <c r="F15" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G15" s="4">
+        <v>5</v>
+      </c>
+      <c r="H15" s="4">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
+    <row r="16" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="30">
-        <f t="shared" si="0"/>
+      <c r="B16" s="1">
+        <v>7</v>
+      </c>
+      <c r="C16" s="33">
+        <f>(D16+E16+F16+G16+H16)/8</f>
         <v>6.875</v>
       </c>
-      <c r="C16" s="4">
+      <c r="D16" s="4">
         <v>15</v>
       </c>
-      <c r="D16" s="4">
-        <v>20</v>
-      </c>
       <c r="E16" s="4">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F16" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G16" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="B17" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C17" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="H16" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="29"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="33"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="33"/>
       <c r="D18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="G18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="H18" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="15" t="s">
+    <row r="19" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="30">
-        <f t="shared" si="0"/>
+      <c r="B19" s="1">
+        <v>7</v>
+      </c>
+      <c r="C19" s="33">
+        <f>(D19+E19+F19+G19+H19)/8</f>
         <v>6.25</v>
       </c>
-      <c r="C19" s="4">
-        <v>10</v>
-      </c>
       <c r="D19" s="4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E19" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F19" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G19" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="15" t="s">
+      <c r="H19" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="30">
-        <f t="shared" si="0"/>
+      <c r="B20" s="1">
+        <v>7</v>
+      </c>
+      <c r="C20" s="33">
+        <f>(D20+E20+F20+G20+H20)/8</f>
         <v>6.875</v>
       </c>
-      <c r="C20" s="4">
-        <v>5</v>
-      </c>
       <c r="D20" s="4">
+        <v>5</v>
+      </c>
+      <c r="E20" s="4">
         <v>15</v>
       </c>
-      <c r="E20" s="4">
+      <c r="F20" s="4">
         <v>30</v>
       </c>
-      <c r="F20" s="4">
-        <v>5</v>
-      </c>
-      <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="15" t="s">
+      <c r="G20" s="4">
+        <v>5</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="30">
-        <f t="shared" si="0"/>
+      <c r="B21" s="1">
+        <v>7</v>
+      </c>
+      <c r="C21" s="33">
+        <f>(D21+E21+F21+G21+H21)/8</f>
         <v>6.875</v>
       </c>
-      <c r="C21" s="4">
-        <v>5</v>
-      </c>
       <c r="D21" s="4">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E21" s="4">
+        <v>20</v>
+      </c>
+      <c r="F21" s="4">
         <v>25</v>
       </c>
-      <c r="F21" s="4">
-        <v>5</v>
-      </c>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="12" t="s">
+      <c r="G21" s="4">
+        <v>5</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="30">
-        <f t="shared" si="0"/>
+      <c r="B22" s="1">
+        <v>11</v>
+      </c>
+      <c r="C22" s="33">
+        <f>(D22+E22+F22+G22+H22)/8</f>
         <v>10.625</v>
       </c>
-      <c r="C22" s="4">
-        <v>10</v>
-      </c>
       <c r="D22" s="4">
+        <v>10</v>
+      </c>
+      <c r="E22" s="4">
         <v>40</v>
       </c>
-      <c r="E22" s="4">
-        <v>10</v>
-      </c>
       <c r="F22" s="4">
+        <v>10</v>
+      </c>
+      <c r="G22" s="4">
         <v>15</v>
       </c>
-      <c r="G22" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="13" t="s">
+      <c r="H22" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="30">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C23" s="4">
+      <c r="B23" s="1">
+        <v>5</v>
+      </c>
+      <c r="C23" s="33">
+        <f>(D23+E23+F23+G23+H23)/8</f>
         <v>5</v>
       </c>
       <c r="D23" s="4">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E23" s="4">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F23" s="4">
         <v>5</v>
@@ -1415,23 +1494,26 @@
       <c r="G23" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="13" t="s">
+      <c r="H23" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="30">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C24" s="4">
+      <c r="B24" s="1">
+        <v>5</v>
+      </c>
+      <c r="C24" s="33">
+        <f>(D24+E24+F24+G24+H24)/8</f>
         <v>5</v>
       </c>
       <c r="D24" s="4">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E24" s="4">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F24" s="4">
         <v>5</v>
@@ -1439,647 +1521,678 @@
       <c r="G24" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="12" t="s">
+      <c r="H24" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C25" s="4"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="33"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="13" t="s">
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="B26" s="30">
-        <f t="shared" si="0"/>
+      <c r="B26" s="1">
+        <v>7</v>
+      </c>
+      <c r="C26" s="33">
+        <f>(D26+E26+F26+G26+H26)/8</f>
         <v>6.875</v>
       </c>
-      <c r="C26" s="4">
-        <v>5</v>
-      </c>
       <c r="D26" s="4">
+        <v>5</v>
+      </c>
+      <c r="E26" s="4">
         <v>25</v>
       </c>
-      <c r="E26" s="4">
-        <v>5</v>
-      </c>
       <c r="F26" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G26" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="13" t="s">
+      <c r="H26" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="30">
-        <f t="shared" si="0"/>
+      <c r="B27" s="1">
+        <v>6</v>
+      </c>
+      <c r="C27" s="33">
+        <f>(D27+E27+F27+G27+H27)/8</f>
         <v>5.625</v>
       </c>
-      <c r="C27" s="4">
-        <v>5</v>
-      </c>
       <c r="D27" s="4">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E27" s="4">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F27" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G27" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="13"/>
-      <c r="B28" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C28" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="H27" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="32"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="33"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>81</v>
       </c>
-      <c r="B29" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C29" s="4"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="33"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-    </row>
-    <row r="30" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="18" t="s">
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B30" s="30">
-        <f t="shared" si="0"/>
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="33">
+        <f>(D30+E30+F30+G30+H30)/8</f>
         <v>8.125</v>
       </c>
-      <c r="C30" s="4">
-        <v>5</v>
-      </c>
       <c r="D30" s="4">
+        <v>5</v>
+      </c>
+      <c r="E30" s="4">
         <v>30</v>
       </c>
-      <c r="E30" s="4">
-        <v>10</v>
-      </c>
       <c r="F30" s="4">
         <v>10</v>
       </c>
       <c r="G30" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="13" t="s">
+      <c r="H30" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="B31" s="30">
-        <f t="shared" si="0"/>
+      <c r="B31" s="1">
+        <v>7</v>
+      </c>
+      <c r="C31" s="33">
+        <f>(D31+E31+F31+G31+H31)/8</f>
         <v>6.875</v>
       </c>
-      <c r="C31" s="4">
-        <v>5</v>
-      </c>
       <c r="D31" s="4">
+        <v>5</v>
+      </c>
+      <c r="E31" s="4">
         <v>25</v>
       </c>
-      <c r="E31" s="4">
-        <v>5</v>
-      </c>
       <c r="F31" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G31" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="13"/>
-      <c r="B32" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C32" s="4"/>
+      <c r="H31" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="32"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="33"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C33" s="4"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="33"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="19" t="s">
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="30">
-        <f t="shared" si="0"/>
+      <c r="B34" s="1">
+        <v>7</v>
+      </c>
+      <c r="C34" s="33">
+        <f>(D34+E34+F34+G34+H34)/8</f>
         <v>6.875</v>
       </c>
-      <c r="C34" s="4">
-        <v>5</v>
-      </c>
       <c r="D34" s="4">
+        <v>5</v>
+      </c>
+      <c r="E34" s="4">
         <v>25</v>
       </c>
-      <c r="E34" s="4">
-        <v>10</v>
-      </c>
       <c r="F34" s="4">
         <v>10</v>
       </c>
       <c r="G34" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="13"/>
-      <c r="B35" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C35" s="4">
-        <v>0</v>
-      </c>
-      <c r="D35" s="4">
-        <v>0</v>
-      </c>
-      <c r="E35" s="4">
-        <v>0</v>
-      </c>
-      <c r="F35" s="4">
-        <v>0</v>
-      </c>
-      <c r="G35" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="13"/>
-      <c r="B36" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C36" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="H34" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="32"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="18"/>
+    </row>
+    <row r="36" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="32"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="33"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
-    </row>
-    <row r="37" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="12" t="s">
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C37" s="4"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="33"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
-    </row>
-    <row r="38" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="13" t="s">
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="B38" s="30">
-        <f t="shared" si="0"/>
+      <c r="B38" s="1">
+        <v>6</v>
+      </c>
+      <c r="C38" s="33">
+        <f>(D38+E38+F38+G38+H38)/8</f>
         <v>5.625</v>
       </c>
-      <c r="C38" s="4">
-        <v>5</v>
-      </c>
       <c r="D38" s="4">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E38" s="4">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F38" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G38" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="30">
-        <f t="shared" si="0"/>
+      <c r="B39" s="1">
+        <v>6</v>
+      </c>
+      <c r="C39" s="33">
+        <f>(D39+E39+F39+G39+H39)/8</f>
         <v>5.625</v>
       </c>
-      <c r="C39" s="4">
-        <v>5</v>
-      </c>
       <c r="D39" s="4">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E39" s="4">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F39" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G39" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="13"/>
-      <c r="B40" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C40" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="H39" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="32"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="33"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
-    </row>
-    <row r="41" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="12" t="s">
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="B41" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C41" s="4"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="33"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
-    </row>
-    <row r="42" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="13" t="s">
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="B42" s="30">
-        <f t="shared" si="0"/>
+      <c r="B42" s="1">
+        <v>7</v>
+      </c>
+      <c r="C42" s="33">
+        <f>(D42+E42+F42+G42+H42)/8</f>
         <v>6.25</v>
       </c>
-      <c r="C42" s="4">
-        <v>5</v>
-      </c>
       <c r="D42" s="4">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E42" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F42" s="4">
         <v>10</v>
       </c>
       <c r="G42" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="B43" s="30">
-        <f t="shared" si="0"/>
+      <c r="B43" s="1">
+        <v>7</v>
+      </c>
+      <c r="C43" s="33">
+        <f>(D43+E43+F43+G43+H43)/8</f>
         <v>6.25</v>
       </c>
-      <c r="C43" s="4">
-        <v>5</v>
-      </c>
       <c r="D43" s="4">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E43" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F43" s="4">
         <v>10</v>
       </c>
       <c r="G43" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H43" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="B44" s="30">
-        <f t="shared" si="0"/>
+      <c r="B44" s="1">
+        <v>7</v>
+      </c>
+      <c r="C44" s="33">
+        <f>(D44+E44+F44+G44+H44)/8</f>
         <v>6.25</v>
       </c>
-      <c r="C44" s="4">
-        <v>5</v>
-      </c>
       <c r="D44" s="4">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E44" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F44" s="4">
         <v>10</v>
       </c>
       <c r="G44" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="13"/>
-      <c r="B45" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C45" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="H44" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="32"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="33"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
-    </row>
-    <row r="46" spans="1:7" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="13"/>
-      <c r="B46" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C46" s="4"/>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="32"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="33"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
-    </row>
-    <row r="47" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B47" s="30"/>
-      <c r="C47" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A47" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="33"/>
       <c r="D47" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="F47" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="G47" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G47" s="6" t="s">
+      <c r="H47" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="17" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B48" s="30">
-        <f t="shared" si="0"/>
+      <c r="B48" s="1">
+        <v>7</v>
+      </c>
+      <c r="C48" s="33">
+        <f>(D48+E48+F48+G48+H48)/8</f>
         <v>6.875</v>
       </c>
-      <c r="C48" s="1">
-        <v>5</v>
-      </c>
       <c r="D48" s="1">
+        <v>5</v>
+      </c>
+      <c r="E48" s="1">
         <v>15</v>
       </c>
-      <c r="E48" s="1">
-        <v>10</v>
-      </c>
       <c r="F48" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G48" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H48" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B49" s="30">
-        <f t="shared" si="0"/>
+      <c r="B49" s="1">
+        <v>9</v>
+      </c>
+      <c r="C49" s="33">
+        <f>(D49+E49+F49+G49+H49)/8</f>
         <v>8.125</v>
       </c>
-      <c r="C49" s="1">
-        <v>5</v>
-      </c>
       <c r="D49" s="1">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E49" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F49" s="1">
+        <v>5</v>
+      </c>
+      <c r="G49" s="1">
         <v>30</v>
       </c>
-      <c r="G49" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="17" t="s">
+      <c r="H49" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B50" s="30">
-        <f t="shared" si="0"/>
+      <c r="B50" s="1">
+        <v>9</v>
+      </c>
+      <c r="C50" s="33">
+        <f>(D50+E50+F50+G50+H50)/8</f>
         <v>8.75</v>
       </c>
-      <c r="C50" s="1">
-        <v>10</v>
-      </c>
       <c r="D50" s="1">
+        <v>10</v>
+      </c>
+      <c r="E50" s="1">
         <v>15</v>
       </c>
-      <c r="E50" s="1">
-        <v>5</v>
-      </c>
       <c r="F50" s="1">
+        <v>5</v>
+      </c>
+      <c r="G50" s="1">
         <v>30</v>
       </c>
-      <c r="G50" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="1"/>
-      <c r="B51" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C51" s="1"/>
+      <c r="H50" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="29"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="33"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7" ht="29" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="2" t="s">
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="1:8" ht="29" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="30"/>
-      <c r="C52" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="B52" s="1"/>
+      <c r="C52" s="33"/>
       <c r="D52" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E52" s="6" t="s">
+      <c r="F52" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F52" s="6" t="s">
+      <c r="G52" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G52" s="6" t="s">
+      <c r="H52" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="17" t="s">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B53" s="30">
-        <f t="shared" si="0"/>
+      <c r="B53" s="1">
+        <v>9</v>
+      </c>
+      <c r="C53" s="33">
+        <f>(D53+E53+F53+G53+H53)/8</f>
         <v>8.125</v>
       </c>
-      <c r="C53" s="1">
+      <c r="D53" s="1">
         <v>15</v>
       </c>
-      <c r="D53" s="1">
-        <v>20</v>
-      </c>
       <c r="E53" s="1">
+        <v>20</v>
+      </c>
+      <c r="F53" s="1">
         <v>15</v>
       </c>
-      <c r="F53" s="1">
-        <v>10</v>
-      </c>
       <c r="G53" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H53" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B54" s="30">
-        <f t="shared" si="0"/>
+      <c r="B54" s="1">
+        <v>8</v>
+      </c>
+      <c r="C54" s="33">
+        <f>(D54+E54+F54+G54+H54)/8</f>
         <v>7.5</v>
       </c>
-      <c r="C54" s="1">
-        <v>20</v>
-      </c>
       <c r="D54" s="1">
         <v>20</v>
       </c>
-      <c r="E54" s="1"/>
+      <c r="E54" s="1">
+        <v>20</v>
+      </c>
       <c r="F54" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G54" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="17" t="s">
+      <c r="H54" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B55" s="30">
-        <f t="shared" si="0"/>
+      <c r="B55" s="1">
+        <v>7</v>
+      </c>
+      <c r="C55" s="33">
+        <f>(D55+E55+F55+G55+H55)/8</f>
         <v>6.25</v>
       </c>
-      <c r="C55" s="1">
-        <v>10</v>
-      </c>
       <c r="D55" s="1">
         <v>10</v>
       </c>
-      <c r="E55" s="1"/>
+      <c r="E55" s="1">
+        <v>10</v>
+      </c>
       <c r="F55" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G55" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H55" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B56" s="30">
-        <f t="shared" si="0"/>
+      <c r="B56" s="1">
+        <v>4</v>
+      </c>
+      <c r="C56" s="33">
+        <f>(D56+E56+F56+G56+H56)/8</f>
         <v>3.75</v>
       </c>
-      <c r="C56" s="1">
+      <c r="D56" s="1">
         <v>15</v>
       </c>
-      <c r="D56" s="1">
-        <v>5</v>
-      </c>
-      <c r="E56" s="1"/>
+      <c r="E56" s="1">
+        <v>5</v>
+      </c>
       <c r="F56" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G56" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="1"/>
+      <c r="H56" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="29"/>
       <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
+      <c r="C57" s="34"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H57" s="1"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B58">
         <f>SUM(B6:B57)</f>
+        <v>222</v>
+      </c>
+      <c r="C58" s="28">
+        <f>SUM(C6:C57)</f>
         <v>209.375</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A2:E2"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2091,8 +2204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:M44"/>
   <sheetViews>
-    <sheetView zoomScale="64" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="64" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2129,12 +2242,12 @@
       <c r="F2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -2146,14 +2259,14 @@
       <c r="C3" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="20">
         <v>25000</v>
       </c>
       <c r="E3" s="8">
-        <f>EDT!C6+EDT!C7+EDT!C8+EDT!C9</f>
+        <f>EDT!D6+EDT!D7+EDT!D8+EDT!D9</f>
         <v>60</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="20">
         <f>D3*E3</f>
         <v>1500000</v>
       </c>
@@ -2180,14 +2293,14 @@
       <c r="C4" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="20">
         <v>22000</v>
       </c>
       <c r="E4" s="8">
-        <f>EDT!D6+EDT!D7+EDT!D8+EDT!D9</f>
+        <f>EDT!E6+EDT!E7+EDT!E8+EDT!E9</f>
         <v>40</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="20">
         <f>D4*E4</f>
         <v>880000</v>
       </c>
@@ -2197,10 +2310,10 @@
       <c r="I4" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="20">
         <v>25000</v>
       </c>
-      <c r="K4" s="21">
+      <c r="K4" s="19">
         <v>4000000</v>
       </c>
     </row>
@@ -2214,14 +2327,14 @@
       <c r="C5" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="20">
         <v>20000</v>
       </c>
       <c r="E5" s="8">
-        <f>EDT!E6+EDT!E7+EDT!E8+EDT!E9</f>
-        <v>10</v>
-      </c>
-      <c r="F5" s="22">
+        <f>EDT!F6+EDT!F7+EDT!F8+EDT!F9</f>
+        <v>10</v>
+      </c>
+      <c r="F5" s="20">
         <f>D5*E5</f>
         <v>200000</v>
       </c>
@@ -2231,10 +2344,10 @@
       <c r="I5" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="J5" s="22">
+      <c r="J5" s="20">
         <v>22000</v>
       </c>
-      <c r="K5" s="22">
+      <c r="K5" s="20">
         <v>3520000</v>
       </c>
     </row>
@@ -2248,14 +2361,14 @@
       <c r="C6" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="20">
         <v>18000</v>
       </c>
       <c r="E6" s="8">
-        <f>EDT!F6+EDT!F7+EDT!F8+EDT!F9</f>
-        <v>20</v>
-      </c>
-      <c r="F6" s="22">
+        <f>EDT!G6+EDT!G7+EDT!G8+EDT!G9</f>
+        <v>20</v>
+      </c>
+      <c r="F6" s="20">
         <f>D6*E6</f>
         <v>360000</v>
       </c>
@@ -2265,10 +2378,10 @@
       <c r="I6" t="s">
         <v>91</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="20">
         <v>20000</v>
       </c>
-      <c r="K6" s="22">
+      <c r="K6" s="20">
         <v>3200000</v>
       </c>
     </row>
@@ -2282,14 +2395,14 @@
       <c r="C7" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="20">
         <v>18000</v>
       </c>
       <c r="E7" s="8">
-        <f>EDT!G6+EDT!G7+EDT!G8+EDT!G9</f>
+        <f>EDT!H6+EDT!H7+EDT!H8+EDT!H9</f>
         <v>15</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="20">
         <f>D7*E7</f>
         <v>270000</v>
       </c>
@@ -2299,22 +2412,22 @@
       <c r="I7" t="s">
         <v>92</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="20">
         <v>18000</v>
       </c>
-      <c r="K7" s="22">
+      <c r="K7" s="20">
         <v>2880000</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="22">
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="20">
         <f>SUM(F3:F7)</f>
         <v>3210000</v>
       </c>
@@ -2324,10 +2437,10 @@
       <c r="I8" t="s">
         <v>93</v>
       </c>
-      <c r="J8" s="22">
+      <c r="J8" s="20">
         <v>18000</v>
       </c>
-      <c r="K8" s="22">
+      <c r="K8" s="20">
         <v>2880000</v>
       </c>
     </row>
@@ -2350,10 +2463,10 @@
       <c r="F11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="H11" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="26"/>
+      <c r="I11" s="24"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -2365,11 +2478,11 @@
       <c r="C12" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="20">
         <v>25000</v>
       </c>
       <c r="E12" s="8">
-        <f>EDT!C12+EDT!C13+EDT!C14+EDT!C15+EDT!C16</f>
+        <f>EDT!D12+EDT!D13+EDT!D14+EDT!D15+EDT!D16</f>
         <v>55</v>
       </c>
       <c r="F12" s="7">
@@ -2394,11 +2507,11 @@
       <c r="C13" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="20">
         <v>22000</v>
       </c>
       <c r="E13" s="8">
-        <f>EDT!D12+EDT!D13+EDT!D14+EDT!D15+EDT!D16</f>
+        <f>EDT!E12+EDT!E13+EDT!E14+EDT!E15+EDT!E16</f>
         <v>115</v>
       </c>
       <c r="F13" s="7">
@@ -2424,11 +2537,11 @@
       <c r="C14" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="20">
         <v>20000</v>
       </c>
       <c r="E14" s="8">
-        <f>EDT!E12+EDT!E13+EDT!E14+EDT!E15+EDT!E16</f>
+        <f>EDT!F12+EDT!F13+EDT!F14+EDT!F15+EDT!F16</f>
         <v>30</v>
       </c>
       <c r="F14" s="7">
@@ -2453,11 +2566,11 @@
       <c r="C15" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="20">
         <v>18000</v>
       </c>
       <c r="E15" s="8">
-        <f>EDT!F12+EDT!F13+EDT!F14+EDT!F15+EDT!F16</f>
+        <f>EDT!G12+EDT!G13+EDT!G14+EDT!G15+EDT!G16</f>
         <v>35</v>
       </c>
       <c r="F15" s="7">
@@ -2482,11 +2595,11 @@
       <c r="C16" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="20">
         <v>18000</v>
       </c>
       <c r="E16" s="8">
-        <f>EDT!G12+EDT!G13+EDT!G14+EDT!G15+EDT!G16</f>
+        <f>EDT!H12+EDT!H13+EDT!H14+EDT!H15+EDT!H16</f>
         <v>60</v>
       </c>
       <c r="F16" s="7">
@@ -2500,15 +2613,18 @@
         <f>F7+F16+F25+F34+F43</f>
         <v>4050000</v>
       </c>
+      <c r="J16">
+        <v>4</v>
+      </c>
     </row>
     <row r="17" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="29"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
       <c r="F17" s="7">
         <f>SUM(F12:F16)</f>
         <v>6215000</v>
@@ -2543,10 +2659,10 @@
       <c r="F20" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="I20" s="26"/>
+      <c r="I20" s="24"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
@@ -2558,11 +2674,11 @@
       <c r="C21" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D21" s="20">
         <v>25000</v>
       </c>
       <c r="E21" s="8">
-        <f>EDT!C19+EDT!C20+EDT!C21+EDT!C22+EDT!C23+EDT!C24+EDT!C26+EDT!C27+EDT!C30+EDT!C31+EDT!C34+EDT!C38+EDT!C39+EDT!C42+EDT!C43+EDT!C44</f>
+        <f>EDT!D19+EDT!D20+EDT!D21+EDT!D22+EDT!D23+EDT!D24+EDT!D26+EDT!D27+EDT!D30+EDT!D31+EDT!D34+EDT!D38+EDT!D39+EDT!D42+EDT!D43+EDT!D44</f>
         <v>90</v>
       </c>
       <c r="F21" s="7">
@@ -2577,7 +2693,7 @@
         <v>3210000</v>
       </c>
       <c r="M21" s="8">
-        <f>EDT!K24+EDT!K25+EDT!K26+EDT!K27+EDT!K30+EDT!K31+EDT!K32+EDT!K33+EDT!K34+EDT!K37+EDT!K38+EDT!K39+EDT!K40+EDT!K41+EDT!K42+EDT!K44+EDT!K45+EDT!K48+EDT!K49+EDT!K52+EDT!K53+EDT!K56+EDT!K57+EDT!K60+EDT!K61+EDT!K62+EDT!K66+EDT!K67+EDT!K68+EDT!K71+EDT!K72+EDT!K73+EDT!K74</f>
+        <f>EDT!L24+EDT!L25+EDT!L26+EDT!L27+EDT!L30+EDT!L31+EDT!L32+EDT!L33+EDT!L34+EDT!L37+EDT!L38+EDT!L39+EDT!L40+EDT!L41+EDT!L42+EDT!L44+EDT!L45+EDT!L48+EDT!L49+EDT!L52+EDT!L53+EDT!L56+EDT!L57+EDT!L60+EDT!L61+EDT!L62+EDT!L66+EDT!L67+EDT!L68+EDT!L71+EDT!L72+EDT!L73+EDT!L74</f>
         <v>0</v>
       </c>
     </row>
@@ -2591,11 +2707,11 @@
       <c r="C22" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22" s="20">
         <v>22000</v>
       </c>
       <c r="E22" s="8">
-        <f>EDT!D19+EDT!D20+EDT!D21+EDT!D22+EDT!D23+EDT!D24+EDT!D26+EDT!D27+EDT!D30+EDT!D31+EDT!D34+EDT!D35+EDT!D38+EDT!D39+EDT!D42+EDT!D43+EDT!D44</f>
+        <f>EDT!E19+EDT!E20+EDT!E21+EDT!E22+EDT!E23+EDT!E24+EDT!E26+EDT!E27+EDT!E30+EDT!E31+EDT!E34+EDT!E35+EDT!E38+EDT!E39+EDT!E42+EDT!E43+EDT!E44</f>
         <v>360</v>
       </c>
       <c r="F22" s="7">
@@ -2620,11 +2736,11 @@
       <c r="C23" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="20">
         <v>20000</v>
       </c>
       <c r="E23" s="8">
-        <f>EDT!E19+EDT!E20+EDT!E21+EDT!E22+EDT!E23+EDT!E24+EDT!E26+EDT!E27+EDT!E30+EDT!E31+EDT!E34+EDT!E35+EDT!E38+EDT!E39+EDT!E42+EDT!E43+EDT!E44</f>
+        <f>EDT!F19+EDT!F20+EDT!F21+EDT!F22+EDT!F23+EDT!F24+EDT!F26+EDT!F27+EDT!F30+EDT!F31+EDT!F34+EDT!F35+EDT!F38+EDT!F39+EDT!F42+EDT!F43+EDT!F44</f>
         <v>160</v>
       </c>
       <c r="F23" s="7">
@@ -2649,11 +2765,11 @@
       <c r="C24" t="s">
         <v>92</v>
       </c>
-      <c r="D24" s="22">
+      <c r="D24" s="20">
         <v>18000</v>
       </c>
       <c r="E24" s="8">
-        <f>EDT!F19+EDT!F20+EDT!F21+EDT!F22+EDT!F23+EDT!F24+EDT!F26+EDT!F27+EDT!F30+EDT!F31+EDT!F34+EDT!F35</f>
+        <f>EDT!G19+EDT!G20+EDT!G21+EDT!G22+EDT!G23+EDT!G24+EDT!G26+EDT!G27+EDT!G30+EDT!G31+EDT!G34+EDT!G35</f>
         <v>90</v>
       </c>
       <c r="F24" s="7">
@@ -2678,11 +2794,11 @@
       <c r="C25" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="20">
         <v>18000</v>
       </c>
       <c r="E25" s="8">
-        <f>EDT!G19+EDT!G20+EDT!G21+EDT!G22+EDT!G23+EDT!G24+EDT!G26+EDT!G27+EDT!G30+EDT!G31+EDT!G34+EDT!G35+EDT!G38+EDT!G39+EDT!G42+EDT!G43+EDT!G44</f>
+        <f>EDT!H19+EDT!H20+EDT!H21+EDT!H22+EDT!H23+EDT!H24+EDT!H26+EDT!H27+EDT!H30+EDT!H31+EDT!H34+EDT!H35+EDT!H38+EDT!H39+EDT!H42+EDT!H43+EDT!H44</f>
         <v>90</v>
       </c>
       <c r="F25" s="7">
@@ -2699,12 +2815,12 @@
     </row>
     <row r="26" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="29"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="27"/>
       <c r="F26" s="7">
         <f>SUM(F21:F25)</f>
         <v>16610000</v>
@@ -2739,7 +2855,7 @@
       <c r="H29" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="I29" s="14">
+      <c r="I29" s="12">
         <v>0.6</v>
       </c>
     </row>
@@ -2753,11 +2869,11 @@
       <c r="C30" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="22">
+      <c r="D30" s="20">
         <v>25000</v>
       </c>
       <c r="E30" s="8">
-        <f>EDT!C48+EDT!C49+EDT!C50</f>
+        <f>EDT!D48+EDT!D49+EDT!D50</f>
         <v>20</v>
       </c>
       <c r="F30" s="7">
@@ -2782,11 +2898,11 @@
       <c r="C31" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="22">
+      <c r="D31" s="20">
         <v>22000</v>
       </c>
       <c r="E31" s="8">
-        <f>EDT!D48+EDT!D49+EDT!D50</f>
+        <f>EDT!E48+EDT!E49+EDT!E50</f>
         <v>50</v>
       </c>
       <c r="F31" s="7">
@@ -2811,11 +2927,11 @@
       <c r="C32" t="s">
         <v>91</v>
       </c>
-      <c r="D32" s="22">
+      <c r="D32" s="20">
         <v>20000</v>
       </c>
       <c r="E32" s="8">
-        <f>EDT!E48+EDT!E49+EDT!E50</f>
+        <f>EDT!F48+EDT!F49+EDT!F50</f>
         <v>20</v>
       </c>
       <c r="F32" s="7">
@@ -2833,11 +2949,11 @@
       <c r="C33" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D33" s="20">
         <v>18000</v>
       </c>
       <c r="E33" s="8">
-        <f>EDT!F48+EDT!F49+EDT!F50</f>
+        <f>EDT!G48+EDT!G49+EDT!G50</f>
         <v>80</v>
       </c>
       <c r="F33" s="7">
@@ -2855,11 +2971,11 @@
       <c r="C34" t="s">
         <v>93</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="20">
         <v>18000</v>
       </c>
       <c r="E34" s="8">
-        <f>EDT!G48+EDT!G49+EDT!G50</f>
+        <f>EDT!H48+EDT!H49+EDT!H50</f>
         <v>20</v>
       </c>
       <c r="F34" s="7">
@@ -2869,12 +2985,12 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="29"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="27"/>
       <c r="F35" s="7">
         <f>SUM(F30:F34)</f>
         <v>3800000</v>
@@ -2910,11 +3026,11 @@
       <c r="C39" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D39" s="22">
+      <c r="D39" s="20">
         <v>25000</v>
       </c>
       <c r="E39" s="8">
-        <f>EDT!C53+EDT!C54+EDT!C55+EDT!C56</f>
+        <f>EDT!D53+EDT!D54+EDT!D55+EDT!D56</f>
         <v>60</v>
       </c>
       <c r="F39" s="7">
@@ -2932,11 +3048,11 @@
       <c r="C40" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D40" s="22">
+      <c r="D40" s="20">
         <v>22000</v>
       </c>
       <c r="E40" s="8">
-        <f>EDT!D53+EDT!D54+EDT!D55+EDT!D56</f>
+        <f>EDT!E53+EDT!E54+EDT!E55+EDT!E56</f>
         <v>55</v>
       </c>
       <c r="F40" s="7">
@@ -2954,11 +3070,11 @@
       <c r="C41" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="22">
+      <c r="D41" s="20">
         <v>20000</v>
       </c>
       <c r="E41" s="8">
-        <f>EDT!E53+EDT!E54+EDT!E55+EDT!E56</f>
+        <f>EDT!F53+EDT!F54+EDT!F55+EDT!F56</f>
         <v>15</v>
       </c>
       <c r="F41" s="7">
@@ -2976,11 +3092,11 @@
       <c r="C42" t="s">
         <v>92</v>
       </c>
-      <c r="D42" s="22">
+      <c r="D42" s="20">
         <v>18000</v>
       </c>
       <c r="E42" s="8">
-        <f>EDT!F53+EDT!F54+EDT!F55+EDT!F56</f>
+        <f>EDT!G53+EDT!G54+EDT!G55+EDT!G56</f>
         <v>35</v>
       </c>
       <c r="F42" s="7">
@@ -2998,11 +3114,11 @@
       <c r="C43" t="s">
         <v>93</v>
       </c>
-      <c r="D43" s="22">
+      <c r="D43" s="20">
         <v>18000</v>
       </c>
       <c r="E43" s="8">
-        <f>EDT!G53+EDT!G54+EDT!G55+EDT!G56</f>
+        <f>EDT!H53+EDT!H54+EDT!H55+EDT!H56</f>
         <v>40</v>
       </c>
       <c r="F43" s="7">
@@ -3012,12 +3128,12 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="29"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="27"/>
       <c r="F44" s="7">
         <f>SUM(F39:F43)</f>
         <v>4360000</v>

</xml_diff>

<commit_message>
(fase1: ajuste presupuesto y caso de uso extendido)
</commit_message>
<xml_diff>
--- a/fase1/Documentacion Proyecto/Matriz EDT.xlsb.xlsx
+++ b/fase1/Documentacion Proyecto/Matriz EDT.xlsb.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\git\Capstone\fase1\Documentacion Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7261F15C-531A-4025-BCAA-84EF27747CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A0E1EA-71E4-4361-B13F-2D526FA4018A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -237,9 +237,6 @@
     <t xml:space="preserve">Margen </t>
   </si>
   <si>
-    <t>UTILIDAD</t>
-  </si>
-  <si>
     <t>PRECIO FINAL</t>
   </si>
   <si>
@@ -325,6 +322,9 @@
   </si>
   <si>
     <t>dias esperados</t>
+  </si>
+  <si>
+    <t>Reserva</t>
   </si>
 </sst>
 </file>
@@ -597,6 +597,18 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -618,18 +630,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares [0]" xfId="1" builtinId="6"/>
@@ -966,43 +966,43 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="J4" s="21" t="s">
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="J4" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="21"/>
+      <c r="K4" s="29"/>
     </row>
     <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>20</v>
@@ -1033,7 +1033,7 @@
       <c r="B6" s="1">
         <v>5</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="26">
         <f>(D6+E6+F6+G6+H6)/8</f>
         <v>4.375</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>20</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.35">
@@ -1066,7 +1066,7 @@
       <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="26">
         <f>(D7+E7+F7+G7+H7)/8</f>
         <v>2.5</v>
       </c>
@@ -1089,17 +1089,17 @@
         <v>21</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="1">
         <v>8</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="26">
         <f>(D8+E8+F8+G8+H8)/8</f>
         <v>7.5</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>22</v>
       </c>
       <c r="K8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.35">
@@ -1132,7 +1132,7 @@
       <c r="B9" s="1">
         <v>4</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="26">
         <f>(D9+E9+F9+G9+H9)/8</f>
         <v>3.75</v>
       </c>
@@ -1155,13 +1155,13 @@
         <v>23</v>
       </c>
       <c r="K9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="29"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="33"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -1171,15 +1171,15 @@
         <v>24</v>
       </c>
       <c r="K10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="33"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="6" t="s">
         <v>20</v>
       </c>
@@ -1203,7 +1203,7 @@
       <c r="B12" s="1">
         <v>9</v>
       </c>
-      <c r="C12" s="33">
+      <c r="C12" s="26">
         <f>(D12+E12+F12+G12+H12)/8</f>
         <v>8.75</v>
       </c>
@@ -1230,7 +1230,7 @@
       <c r="B13" s="1">
         <v>8</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13" s="26">
         <f>(D13+E13+F13+G13+H13)/8</f>
         <v>7.5</v>
       </c>
@@ -1257,7 +1257,7 @@
       <c r="B14" s="1">
         <v>7</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C14" s="26">
         <f>(D14+E14+F14+G14+H14)/8</f>
         <v>6.875</v>
       </c>
@@ -1284,7 +1284,7 @@
       <c r="B15" s="1">
         <v>7</v>
       </c>
-      <c r="C15" s="33">
+      <c r="C15" s="26">
         <f>(D15+E15+F15+G15+H15)/8</f>
         <v>6.875</v>
       </c>
@@ -1311,7 +1311,7 @@
       <c r="B16" s="1">
         <v>7</v>
       </c>
-      <c r="C16" s="33">
+      <c r="C16" s="26">
         <f>(D16+E16+F16+G16+H16)/8</f>
         <v>6.875</v>
       </c>
@@ -1332,9 +1332,9 @@
       </c>
     </row>
     <row r="17" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="29"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="33"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -1342,11 +1342,11 @@
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="23" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="33"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="6" t="s">
         <v>20</v>
       </c>
@@ -1370,8 +1370,8 @@
       <c r="B19" s="1">
         <v>7</v>
       </c>
-      <c r="C19" s="33">
-        <f>(D19+E19+F19+G19+H19)/8</f>
+      <c r="C19" s="26">
+        <f t="shared" ref="C19:C24" si="0">(D19+E19+F19+G19+H19)/8</f>
         <v>6.25</v>
       </c>
       <c r="D19" s="4">
@@ -1392,13 +1392,13 @@
     </row>
     <row r="20" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" s="1">
         <v>7</v>
       </c>
-      <c r="C20" s="33">
-        <f>(D20+E20+F20+G20+H20)/8</f>
+      <c r="C20" s="26">
+        <f t="shared" si="0"/>
         <v>6.875</v>
       </c>
       <c r="D20" s="4">
@@ -1419,13 +1419,13 @@
     </row>
     <row r="21" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" s="1">
         <v>7</v>
       </c>
-      <c r="C21" s="33">
-        <f>(D21+E21+F21+G21+H21)/8</f>
+      <c r="C21" s="26">
+        <f t="shared" si="0"/>
         <v>6.875</v>
       </c>
       <c r="D21" s="4">
@@ -1445,14 +1445,14 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="31" t="s">
-        <v>72</v>
+      <c r="A22" s="24" t="s">
+        <v>71</v>
       </c>
       <c r="B22" s="1">
         <v>11</v>
       </c>
-      <c r="C22" s="33">
-        <f>(D22+E22+F22+G22+H22)/8</f>
+      <c r="C22" s="26">
+        <f t="shared" si="0"/>
         <v>10.625</v>
       </c>
       <c r="D22" s="4">
@@ -1472,41 +1472,41 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="1">
+        <v>5</v>
+      </c>
+      <c r="C23" s="26">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D23" s="4">
+        <v>5</v>
+      </c>
+      <c r="E23" s="4">
+        <v>20</v>
+      </c>
+      <c r="F23" s="4">
+        <v>5</v>
+      </c>
+      <c r="G23" s="4">
+        <v>5</v>
+      </c>
+      <c r="H23" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="1">
-        <v>5</v>
-      </c>
-      <c r="C23" s="33">
-        <f>(D23+E23+F23+G23+H23)/8</f>
-        <v>5</v>
-      </c>
-      <c r="D23" s="4">
-        <v>5</v>
-      </c>
-      <c r="E23" s="4">
-        <v>20</v>
-      </c>
-      <c r="F23" s="4">
-        <v>5</v>
-      </c>
-      <c r="G23" s="4">
-        <v>5</v>
-      </c>
-      <c r="H23" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="32" t="s">
-        <v>74</v>
-      </c>
       <c r="B24" s="1">
         <v>5</v>
       </c>
-      <c r="C24" s="33">
-        <f>(D24+E24+F24+G24+H24)/8</f>
+      <c r="C24" s="26">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D24" s="4">
@@ -1526,11 +1526,11 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="31" t="s">
-        <v>78</v>
+      <c r="A25" s="24" t="s">
+        <v>77</v>
       </c>
       <c r="B25" s="1"/>
-      <c r="C25" s="33"/>
+      <c r="C25" s="26"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -1538,13 +1538,13 @@
       <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="32" t="s">
-        <v>79</v>
+      <c r="A26" s="25" t="s">
+        <v>78</v>
       </c>
       <c r="B26" s="1">
         <v>7</v>
       </c>
-      <c r="C26" s="33">
+      <c r="C26" s="26">
         <f>(D26+E26+F26+G26+H26)/8</f>
         <v>6.875</v>
       </c>
@@ -1565,13 +1565,13 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="32" t="s">
-        <v>80</v>
+      <c r="A27" s="25" t="s">
+        <v>79</v>
       </c>
       <c r="B27" s="1">
         <v>6</v>
       </c>
-      <c r="C27" s="33">
+      <c r="C27" s="26">
         <f>(D27+E27+F27+G27+H27)/8</f>
         <v>5.625</v>
       </c>
@@ -1592,9 +1592,9 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="32"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="33"/>
+      <c r="C28" s="26"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -1603,10 +1603,10 @@
     </row>
     <row r="29" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B29" s="1"/>
-      <c r="C29" s="33"/>
+      <c r="C29" s="26"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -1615,12 +1615,12 @@
     </row>
     <row r="30" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A30" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B30" s="1">
         <v>9</v>
       </c>
-      <c r="C30" s="33">
+      <c r="C30" s="26">
         <f>(D30+E30+F30+G30+H30)/8</f>
         <v>8.125</v>
       </c>
@@ -1641,13 +1641,13 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="32" t="s">
-        <v>83</v>
+      <c r="A31" s="25" t="s">
+        <v>82</v>
       </c>
       <c r="B31" s="1">
         <v>7</v>
       </c>
-      <c r="C31" s="33">
+      <c r="C31" s="26">
         <f>(D31+E31+F31+G31+H31)/8</f>
         <v>6.875</v>
       </c>
@@ -1668,9 +1668,9 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="32"/>
+      <c r="A32" s="25"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="33"/>
+      <c r="C32" s="26"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -1679,10 +1679,10 @@
     </row>
     <row r="33" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B33" s="1"/>
-      <c r="C33" s="33"/>
+      <c r="C33" s="26"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -1691,12 +1691,12 @@
     </row>
     <row r="34" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B34" s="1">
         <v>7</v>
       </c>
-      <c r="C34" s="33">
+      <c r="C34" s="26">
         <f>(D34+E34+F34+G34+H34)/8</f>
         <v>6.875</v>
       </c>
@@ -1717,9 +1717,9 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="32"/>
+      <c r="A35" s="25"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="33"/>
+      <c r="C35" s="26"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -1727,9 +1727,9 @@
       <c r="H35" s="18"/>
     </row>
     <row r="36" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="32"/>
+      <c r="A36" s="25"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="33"/>
+      <c r="C36" s="26"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -1737,11 +1737,11 @@
       <c r="H36" s="4"/>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="24" t="s">
         <v>62</v>
       </c>
       <c r="B37" s="1"/>
-      <c r="C37" s="33"/>
+      <c r="C37" s="26"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -1749,13 +1749,13 @@
       <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="25" t="s">
         <v>63</v>
       </c>
       <c r="B38" s="1">
         <v>6</v>
       </c>
-      <c r="C38" s="33">
+      <c r="C38" s="26">
         <f>(D38+E38+F38+G38+H38)/8</f>
         <v>5.625</v>
       </c>
@@ -1776,13 +1776,13 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="25" t="s">
         <v>64</v>
       </c>
       <c r="B39" s="1">
         <v>6</v>
       </c>
-      <c r="C39" s="33">
+      <c r="C39" s="26">
         <f>(D39+E39+F39+G39+H39)/8</f>
         <v>5.625</v>
       </c>
@@ -1803,9 +1803,9 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="32"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="33"/>
+      <c r="C40" s="26"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
@@ -1813,11 +1813,11 @@
       <c r="H40" s="4"/>
     </row>
     <row r="41" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="31" t="s">
-        <v>71</v>
+      <c r="A41" s="24" t="s">
+        <v>70</v>
       </c>
       <c r="B41" s="1"/>
-      <c r="C41" s="33"/>
+      <c r="C41" s="26"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -1825,13 +1825,13 @@
       <c r="H41" s="4"/>
     </row>
     <row r="42" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="32" t="s">
-        <v>86</v>
+      <c r="A42" s="25" t="s">
+        <v>85</v>
       </c>
       <c r="B42" s="1">
         <v>7</v>
       </c>
-      <c r="C42" s="33">
+      <c r="C42" s="26">
         <f>(D42+E42+F42+G42+H42)/8</f>
         <v>6.25</v>
       </c>
@@ -1852,13 +1852,13 @@
       </c>
     </row>
     <row r="43" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="32" t="s">
-        <v>87</v>
+      <c r="A43" s="25" t="s">
+        <v>86</v>
       </c>
       <c r="B43" s="1">
         <v>7</v>
       </c>
-      <c r="C43" s="33">
+      <c r="C43" s="26">
         <f>(D43+E43+F43+G43+H43)/8</f>
         <v>6.25</v>
       </c>
@@ -1879,13 +1879,13 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="32" t="s">
-        <v>88</v>
+      <c r="A44" s="25" t="s">
+        <v>87</v>
       </c>
       <c r="B44" s="1">
         <v>7</v>
       </c>
-      <c r="C44" s="33">
+      <c r="C44" s="26">
         <f>(D44+E44+F44+G44+H44)/8</f>
         <v>6.25</v>
       </c>
@@ -1906,9 +1906,9 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="32"/>
+      <c r="A45" s="25"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="33"/>
+      <c r="C45" s="26"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
@@ -1916,9 +1916,9 @@
       <c r="H45" s="4"/>
     </row>
     <row r="46" spans="1:8" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="32"/>
+      <c r="A46" s="25"/>
       <c r="B46" s="1"/>
-      <c r="C46" s="33"/>
+      <c r="C46" s="26"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
@@ -1926,11 +1926,11 @@
       <c r="H46" s="4"/>
     </row>
     <row r="47" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="30" t="s">
+      <c r="A47" s="23" t="s">
         <v>10</v>
       </c>
       <c r="B47" s="1"/>
-      <c r="C47" s="33"/>
+      <c r="C47" s="26"/>
       <c r="D47" s="6" t="s">
         <v>20</v>
       </c>
@@ -1954,7 +1954,7 @@
       <c r="B48" s="1">
         <v>7</v>
       </c>
-      <c r="C48" s="33">
+      <c r="C48" s="26">
         <f>(D48+E48+F48+G48+H48)/8</f>
         <v>6.875</v>
       </c>
@@ -1981,7 +1981,7 @@
       <c r="B49" s="1">
         <v>9</v>
       </c>
-      <c r="C49" s="33">
+      <c r="C49" s="26">
         <f>(D49+E49+F49+G49+H49)/8</f>
         <v>8.125</v>
       </c>
@@ -2008,7 +2008,7 @@
       <c r="B50" s="1">
         <v>9</v>
       </c>
-      <c r="C50" s="33">
+      <c r="C50" s="26">
         <f>(D50+E50+F50+G50+H50)/8</f>
         <v>8.75</v>
       </c>
@@ -2029,9 +2029,9 @@
       </c>
     </row>
     <row r="51" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="29"/>
+      <c r="A51" s="22"/>
       <c r="B51" s="1"/>
-      <c r="C51" s="33"/>
+      <c r="C51" s="26"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -2039,11 +2039,11 @@
       <c r="H51" s="1"/>
     </row>
     <row r="52" spans="1:8" ht="29" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="30" t="s">
+      <c r="A52" s="23" t="s">
         <v>3</v>
       </c>
       <c r="B52" s="1"/>
-      <c r="C52" s="33"/>
+      <c r="C52" s="26"/>
       <c r="D52" s="6" t="s">
         <v>20</v>
       </c>
@@ -2067,7 +2067,7 @@
       <c r="B53" s="1">
         <v>9</v>
       </c>
-      <c r="C53" s="33">
+      <c r="C53" s="26">
         <f>(D53+E53+F53+G53+H53)/8</f>
         <v>8.125</v>
       </c>
@@ -2089,12 +2089,12 @@
     </row>
     <row r="54" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A54" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B54" s="1">
         <v>8</v>
       </c>
-      <c r="C54" s="33">
+      <c r="C54" s="26">
         <f>(D54+E54+F54+G54+H54)/8</f>
         <v>7.5</v>
       </c>
@@ -2116,12 +2116,12 @@
     </row>
     <row r="55" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A55" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B55" s="1">
         <v>7</v>
       </c>
-      <c r="C55" s="33">
+      <c r="C55" s="26">
         <f>(D55+E55+F55+G55+H55)/8</f>
         <v>6.25</v>
       </c>
@@ -2148,7 +2148,7 @@
       <c r="B56" s="1">
         <v>4</v>
       </c>
-      <c r="C56" s="33">
+      <c r="C56" s="26">
         <f>(D56+E56+F56+G56+H56)/8</f>
         <v>3.75</v>
       </c>
@@ -2169,9 +2169,9 @@
       </c>
     </row>
     <row r="57" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="29"/>
+      <c r="A57" s="22"/>
       <c r="B57" s="1"/>
-      <c r="C57" s="34"/>
+      <c r="C57" s="27"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -2183,7 +2183,7 @@
         <f>SUM(B6:B57)</f>
         <v>222</v>
       </c>
-      <c r="C58" s="28">
+      <c r="C58" s="21">
         <f>SUM(C6:C57)</f>
         <v>209.375</v>
       </c>
@@ -2205,7 +2205,7 @@
   <dimension ref="A2:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="64" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2242,12 +2242,12 @@
       <c r="F2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -2257,7 +2257,7 @@
         <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3" s="20">
         <v>25000</v>
@@ -2291,7 +2291,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D4" s="20">
         <v>22000</v>
@@ -2308,7 +2308,7 @@
         <v>20</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J4" s="20">
         <v>25000</v>
@@ -2325,7 +2325,7 @@
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5" s="20">
         <v>20000</v>
@@ -2342,7 +2342,7 @@
         <v>21</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J5" s="20">
         <v>22000</v>
@@ -2359,7 +2359,7 @@
         <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D6" s="20">
         <v>18000</v>
@@ -2376,7 +2376,7 @@
         <v>55</v>
       </c>
       <c r="I6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J6" s="20">
         <v>20000</v>
@@ -2393,7 +2393,7 @@
         <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" s="20">
         <v>18000</v>
@@ -2410,7 +2410,7 @@
         <v>52</v>
       </c>
       <c r="I7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J7" s="20">
         <v>18000</v>
@@ -2421,12 +2421,12 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="27"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="35"/>
       <c r="F8" s="20">
         <f>SUM(F3:F7)</f>
         <v>3210000</v>
@@ -2435,7 +2435,7 @@
         <v>24</v>
       </c>
       <c r="I8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J8" s="20">
         <v>18000</v>
@@ -2463,10 +2463,10 @@
       <c r="F11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="24"/>
+      <c r="I11" s="32"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -2476,7 +2476,7 @@
         <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D12" s="20">
         <v>25000</v>
@@ -2505,7 +2505,7 @@
         <v>21</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D13" s="20">
         <v>22000</v>
@@ -2535,7 +2535,7 @@
         <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D14" s="20">
         <v>20000</v>
@@ -2564,7 +2564,7 @@
         <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D15" s="20">
         <v>18000</v>
@@ -2593,7 +2593,7 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D16" s="20">
         <v>18000</v>
@@ -2619,12 +2619,12 @@
     </row>
     <row r="17" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="27"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="35"/>
       <c r="F17" s="7">
         <f>SUM(F12:F16)</f>
         <v>6215000</v>
@@ -2659,10 +2659,10 @@
       <c r="F20" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="23" t="s">
+      <c r="H20" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="I20" s="24"/>
+      <c r="I20" s="32"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
@@ -2672,7 +2672,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D21" s="20">
         <v>25000</v>
@@ -2705,7 +2705,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D22" s="20">
         <v>22000</v>
@@ -2734,7 +2734,7 @@
         <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D23" s="20">
         <v>20000</v>
@@ -2763,7 +2763,7 @@
         <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D24" s="20">
         <v>18000</v>
@@ -2792,7 +2792,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D25" s="20">
         <v>18000</v>
@@ -2815,12 +2815,12 @@
     </row>
     <row r="26" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="27"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="35"/>
       <c r="F26" s="7">
         <f>SUM(F21:F25)</f>
         <v>16610000</v>
@@ -2856,7 +2856,7 @@
         <v>65</v>
       </c>
       <c r="I29" s="12">
-        <v>0.6</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
@@ -2867,7 +2867,7 @@
         <v>20</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D30" s="20">
         <v>25000</v>
@@ -2881,11 +2881,11 @@
         <v>500000</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="I30" s="7">
         <f>I26*I29</f>
-        <v>20517000</v>
+        <v>4103400</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
@@ -2896,7 +2896,7 @@
         <v>21</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D31" s="20">
         <v>22000</v>
@@ -2910,11 +2910,11 @@
         <v>1100000</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I31" s="7">
         <f>I26+I30</f>
-        <v>54712000</v>
+        <v>38298400</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
@@ -2925,7 +2925,7 @@
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D32" s="20">
         <v>20000</v>
@@ -2947,7 +2947,7 @@
         <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D33" s="20">
         <v>18000</v>
@@ -2969,7 +2969,7 @@
         <v>24</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D34" s="20">
         <v>18000</v>
@@ -2985,12 +2985,12 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="27"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="35"/>
       <c r="F35" s="7">
         <f>SUM(F30:F34)</f>
         <v>3800000</v>
@@ -3024,7 +3024,7 @@
         <v>20</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D39" s="20">
         <v>25000</v>
@@ -3046,7 +3046,7 @@
         <v>21</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D40" s="20">
         <v>22000</v>
@@ -3068,7 +3068,7 @@
         <v>31</v>
       </c>
       <c r="C41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D41" s="20">
         <v>20000</v>
@@ -3090,7 +3090,7 @@
         <v>52</v>
       </c>
       <c r="C42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D42" s="20">
         <v>18000</v>
@@ -3112,7 +3112,7 @@
         <v>24</v>
       </c>
       <c r="C43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D43" s="20">
         <v>18000</v>
@@ -3128,12 +3128,12 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
-      <c r="B44" s="25" t="s">
+      <c r="B44" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="27"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="35"/>
       <c r="F44" s="7">
         <f>SUM(F39:F43)</f>
         <v>4360000</v>

</xml_diff>